<commit_message>
excel del 12 de noviembre
</commit_message>
<xml_diff>
--- a/m1/unidad3/Practicas/20191111/datos practica7.xlsx
+++ b/m1/unidad3/Practicas/20191111/datos practica7.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="5" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="5" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="4" r:id="rId1"/>
@@ -65,6 +65,7 @@
     <definedName name="apellido1">'[2]27'!$C$15:$C$22</definedName>
     <definedName name="aprobado">[3]Ejercicio21!$I$22</definedName>
     <definedName name="aprobado1">[4]Ejercicio21!$I$22</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="29">'10'!$K$37:$Q$37</definedName>
     <definedName name="_xlnm.Extract" localSheetId="14">'4'!$A$18</definedName>
     <definedName name="_xlnm.Extract" localSheetId="22">'6-1'!$G$31:$J$31</definedName>
     <definedName name="_xlnm.Extract" localSheetId="24">'7-1'!$H$6:$M$6</definedName>
@@ -98,7 +99,7 @@
     <definedName name="Comida" localSheetId="25">#REF!</definedName>
     <definedName name="Comida" localSheetId="27">#REF!</definedName>
     <definedName name="Comida">#REF!</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="29">'10'!$B$38:$B$39</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="29">'10'!$K$33:$M$35</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="14">'4'!$F$1:$F$12</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="22">'6-1'!$G$27:$G$29</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="24">'7-1'!$H$3:$I$4</definedName>
@@ -162,10 +163,10 @@
   <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="7" r:id="rId35"/>
-    <pivotCache cacheId="16" r:id="rId36"/>
-    <pivotCache cacheId="23" r:id="rId37"/>
-    <pivotCache cacheId="46" r:id="rId38"/>
-    <pivotCache cacheId="38" r:id="rId39"/>
+    <pivotCache cacheId="8" r:id="rId36"/>
+    <pivotCache cacheId="9" r:id="rId37"/>
+    <pivotCache cacheId="10" r:id="rId38"/>
+    <pivotCache cacheId="11" r:id="rId39"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -205,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="364">
   <si>
     <t>Código</t>
   </si>
@@ -1258,6 +1259,45 @@
   </si>
   <si>
     <t>Diez mejores que no sean de la Norte</t>
+  </si>
+  <si>
+    <t>Diez mejores empleados que no son de la zona Norte</t>
+  </si>
+  <si>
+    <t>Dos empleados de la zona Sur con menos ventas</t>
+  </si>
+  <si>
+    <t>Envíos urgentes</t>
+  </si>
+  <si>
+    <t>Criterios</t>
+  </si>
+  <si>
+    <t>Envíos urgentes a Canadá</t>
+  </si>
+  <si>
+    <t>Menos de 200kg con precio superior a 100€</t>
+  </si>
+  <si>
+    <t>&lt;200</t>
+  </si>
+  <si>
+    <t>&gt;100</t>
+  </si>
+  <si>
+    <t>Envíos normales con peso superior o igual a 250</t>
+  </si>
+  <si>
+    <t>&gt;=250</t>
+  </si>
+  <si>
+    <t>Envíos de Canadá y de España con precio entre 150 y 300</t>
+  </si>
+  <si>
+    <t>&gt;=150</t>
+  </si>
+  <si>
+    <t>&lt;=300</t>
   </si>
 </sst>
 </file>
@@ -2020,9 +2060,6 @@
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2032,9 +2069,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2050,6 +2084,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma [0]" xfId="1"/>
@@ -2075,13 +2113,13 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="179" formatCode="0.000"/>
+      <numFmt numFmtId="174" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="178" formatCode="0.0000"/>
+      <numFmt numFmtId="175" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.00000"/>
+      <numFmt numFmtId="176" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2090,25 +2128,25 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode="0.00000000"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="175" formatCode="0.0000000"/>
+      <numFmt numFmtId="174" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="0.000000"/>
+      <numFmt numFmtId="175" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.00000"/>
+      <numFmt numFmtId="176" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="178" formatCode="0.0000"/>
+      <numFmt numFmtId="177" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="179" formatCode="0.000"/>
+      <numFmt numFmtId="178" formatCode="0.0000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="179" formatCode="0.00000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5495,7 +5533,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica10" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica10" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0">
   <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" compact="0" outline="0" showAll="0">
@@ -5598,7 +5636,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica11" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="SECTOR">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica11" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="SECTOR">
   <location ref="A3:C26" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -5734,7 +5772,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica12" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica12" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" numFmtId="167" showAll="0">
@@ -5852,7 +5890,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica13" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica13" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" numFmtId="167" showAll="0">
@@ -5978,7 +6016,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica14" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica14" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="167" showAll="0">
@@ -6135,7 +6173,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica15" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Departamento">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica15" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Departamento">
   <location ref="A3:D11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -6263,7 +6301,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica16" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica16" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:F34" firstHeaderRow="0" firstDataRow="1" firstDataCol="4"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -6815,25 +6853,25 @@
     <dataField name="Promedio de Puntos" fld="3" subtotal="average" baseField="0" baseItem="1041008" numFmtId="2"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="8">
+    <format dxfId="14">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="11">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="14">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -6847,7 +6885,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="Departamento">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="Departamento">
   <location ref="B6:C10" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -6895,7 +6933,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -6976,7 +7014,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -7064,7 +7102,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -7146,7 +7184,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica9" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica9" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -7858,7 +7896,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>257</v>
       </c>
     </row>
@@ -7886,16 +7924,16 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="115">
+      <c r="B5" s="113">
         <v>841.41694613729521</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115">
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="113">
         <v>2404.0484175351294</v>
       </c>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115">
+      <c r="F5" s="113"/>
+      <c r="G5" s="113">
         <v>2404.0484175351294</v>
       </c>
     </row>
@@ -7903,18 +7941,18 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="115"/>
-      <c r="C6" s="115">
+      <c r="B6" s="113"/>
+      <c r="C6" s="113">
         <v>661.11331482216053</v>
       </c>
-      <c r="D6" s="115">
+      <c r="D6" s="113">
         <v>1262.1254192059428</v>
       </c>
-      <c r="E6" s="115">
+      <c r="E6" s="113">
         <v>2554.301443631075</v>
       </c>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115">
+      <c r="F6" s="113"/>
+      <c r="G6" s="113">
         <v>2554.301443631075</v>
       </c>
     </row>
@@ -7922,18 +7960,18 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="115"/>
-      <c r="C7" s="115">
+      <c r="B7" s="113"/>
+      <c r="C7" s="113">
         <v>721.21452526053872</v>
       </c>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115">
+      <c r="D7" s="113"/>
+      <c r="E7" s="113">
         <v>2404.0484175351294</v>
       </c>
-      <c r="F7" s="115">
+      <c r="F7" s="113">
         <v>1803.0363131513468</v>
       </c>
-      <c r="G7" s="115">
+      <c r="G7" s="113">
         <v>2404.0484175351294</v>
       </c>
     </row>
@@ -8376,7 +8414,7 @@
       <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="107">
         <v>4</v>
       </c>
     </row>
@@ -8384,7 +8422,7 @@
       <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="107">
         <v>2</v>
       </c>
     </row>
@@ -8392,7 +8430,7 @@
       <c r="A6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="108">
+      <c r="B6" s="107">
         <v>4</v>
       </c>
     </row>
@@ -8400,7 +8438,7 @@
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="108">
+      <c r="B7" s="107">
         <v>3</v>
       </c>
     </row>
@@ -8408,7 +8446,7 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="108">
+      <c r="B8" s="107">
         <v>4</v>
       </c>
     </row>
@@ -8416,7 +8454,7 @@
       <c r="A9" t="s">
         <v>246</v>
       </c>
-      <c r="B9" s="108">
+      <c r="B9" s="107">
         <v>17</v>
       </c>
     </row>
@@ -8445,10 +8483,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="108" t="s">
         <v>266</v>
       </c>
       <c r="C3" t="s">
@@ -8462,13 +8500,13 @@
       <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="107">
         <v>51</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="107">
         <v>-27.9</v>
       </c>
-      <c r="D4" s="108">
+      <c r="D4" s="107">
         <v>-113.23</v>
       </c>
     </row>
@@ -8476,13 +8514,13 @@
       <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="107">
         <v>19</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="107">
         <v>-61.254999999999995</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D5" s="107">
         <v>-88</v>
       </c>
     </row>
@@ -8490,13 +8528,13 @@
       <c r="A6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="108">
+      <c r="B6" s="107">
         <v>38</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="107">
         <v>38.434999999999995</v>
       </c>
-      <c r="D6" s="108">
+      <c r="D6" s="107">
         <v>-76.900000000000006</v>
       </c>
     </row>
@@ -8504,13 +8542,13 @@
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="108">
+      <c r="B7" s="107">
         <v>17</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <v>3.26</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D7" s="107">
         <v>-50.879999999999995</v>
       </c>
     </row>
@@ -8518,13 +8556,13 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="108">
+      <c r="B8" s="107">
         <v>28</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>-39.267499999999998</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D8" s="107">
         <v>-127.83000000000001</v>
       </c>
     </row>
@@ -8532,13 +8570,13 @@
       <c r="A9" t="s">
         <v>246</v>
       </c>
-      <c r="B9" s="108">
+      <c r="B9" s="107">
         <v>153</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="107">
         <v>-13.391764705882354</v>
       </c>
-      <c r="D9" s="108">
+      <c r="D9" s="107">
         <v>-456.84</v>
       </c>
     </row>
@@ -8563,10 +8601,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="104" t="s">
         <v>69</v>
       </c>
       <c r="C3" t="s">
@@ -8580,7 +8618,7 @@
       <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="107">
         <v>39.25</v>
       </c>
     </row>
@@ -8588,7 +8626,7 @@
       <c r="B5" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="107">
         <v>23.62</v>
       </c>
     </row>
@@ -8596,7 +8634,7 @@
       <c r="B6" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="107">
         <v>8.32</v>
       </c>
     </row>
@@ -8604,7 +8642,7 @@
       <c r="B7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <v>5.54</v>
       </c>
     </row>
@@ -8612,7 +8650,7 @@
       <c r="A8" t="s">
         <v>260</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>19.182500000000001</v>
       </c>
     </row>
@@ -8623,7 +8661,7 @@
       <c r="B9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="107">
         <v>7.69</v>
       </c>
     </row>
@@ -8631,7 +8669,7 @@
       <c r="B10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="107">
         <v>9.4</v>
       </c>
     </row>
@@ -8639,7 +8677,7 @@
       <c r="A11" t="s">
         <v>261</v>
       </c>
-      <c r="C11" s="108">
+      <c r="C11" s="107">
         <v>8.5449999999999999</v>
       </c>
     </row>
@@ -8650,7 +8688,7 @@
       <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="108">
+      <c r="C12" s="107">
         <v>13.57</v>
       </c>
     </row>
@@ -8658,7 +8696,7 @@
       <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="108">
+      <c r="C13" s="107">
         <v>29.7</v>
       </c>
     </row>
@@ -8666,7 +8704,7 @@
       <c r="B14" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="108">
+      <c r="C14" s="107">
         <v>20.47</v>
       </c>
     </row>
@@ -8674,7 +8712,7 @@
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="108">
+      <c r="C15" s="107">
         <v>25.9</v>
       </c>
     </row>
@@ -8682,7 +8720,7 @@
       <c r="A16" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="108">
+      <c r="C16" s="107">
         <v>22.409999999999997</v>
       </c>
     </row>
@@ -8693,7 +8731,7 @@
       <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="108">
+      <c r="C17" s="107">
         <v>5.4</v>
       </c>
     </row>
@@ -8701,7 +8739,7 @@
       <c r="B18" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="108">
+      <c r="C18" s="107">
         <v>18.13</v>
       </c>
     </row>
@@ -8709,7 +8747,7 @@
       <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="108">
+      <c r="C19" s="107">
         <v>1.31</v>
       </c>
     </row>
@@ -8717,7 +8755,7 @@
       <c r="A20" t="s">
         <v>263</v>
       </c>
-      <c r="C20" s="108">
+      <c r="C20" s="107">
         <v>8.2799999999999994</v>
       </c>
     </row>
@@ -8728,7 +8766,7 @@
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="108">
+      <c r="C21" s="107">
         <v>9.61</v>
       </c>
     </row>
@@ -8736,7 +8774,7 @@
       <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="108">
+      <c r="C22" s="107">
         <v>5.45</v>
       </c>
     </row>
@@ -8744,7 +8782,7 @@
       <c r="B23" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="108">
+      <c r="C23" s="107">
         <v>6.21</v>
       </c>
     </row>
@@ -8752,7 +8790,7 @@
       <c r="B24" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="108">
+      <c r="C24" s="107">
         <v>4.21</v>
       </c>
     </row>
@@ -8760,7 +8798,7 @@
       <c r="A25" t="s">
         <v>264</v>
       </c>
-      <c r="C25" s="108">
+      <c r="C25" s="107">
         <v>6.37</v>
       </c>
     </row>
@@ -8768,7 +8806,7 @@
       <c r="A26" t="s">
         <v>246</v>
       </c>
-      <c r="C26" s="108">
+      <c r="C26" s="107">
         <v>13.751764705882355</v>
       </c>
     </row>
@@ -9162,66 +9200,66 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="114" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="114" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="114" t="s">
         <v>279</v>
       </c>
-      <c r="B6" s="108">
+      <c r="B6" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="114" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="108">
+      <c r="B7" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="114" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="108">
+      <c r="B8" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="114" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="108">
+      <c r="B9" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="114" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B10" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="B11" s="108">
+      <c r="B11" s="107">
         <v>11</v>
       </c>
     </row>
@@ -9246,7 +9284,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>282</v>
       </c>
     </row>
@@ -9265,116 +9303,116 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="114" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="107">
         <v>1</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="107">
         <v>1</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D5" s="107">
         <v>1</v>
       </c>
-      <c r="E5" s="108">
+      <c r="E5" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="114" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108">
+      <c r="B6" s="107"/>
+      <c r="C6" s="107">
         <v>2</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108">
+      <c r="D6" s="107"/>
+      <c r="E6" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="114" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108">
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107">
         <v>1</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="114" t="s">
         <v>274</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108">
+      <c r="B8" s="107"/>
+      <c r="C8" s="107">
         <v>1</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108">
+      <c r="D8" s="107"/>
+      <c r="E8" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="114" t="s">
         <v>275</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108">
+      <c r="B9" s="107"/>
+      <c r="C9" s="107">
         <v>1</v>
       </c>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108">
+      <c r="D9" s="107"/>
+      <c r="E9" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="114" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108">
+      <c r="B10" s="107"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="107">
         <v>1</v>
       </c>
-      <c r="E10" s="108">
+      <c r="E10" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="114" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108">
+      <c r="B11" s="107"/>
+      <c r="C11" s="107">
         <v>1</v>
       </c>
-      <c r="D11" s="108">
+      <c r="D11" s="107">
         <v>1</v>
       </c>
-      <c r="E11" s="108">
+      <c r="E11" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="B12" s="108">
+      <c r="B12" s="107">
         <v>1</v>
       </c>
-      <c r="C12" s="108">
+      <c r="C12" s="107">
         <v>6</v>
       </c>
-      <c r="D12" s="108">
+      <c r="D12" s="107">
         <v>4</v>
       </c>
-      <c r="E12" s="108">
+      <c r="E12" s="107">
         <v>11</v>
       </c>
     </row>
@@ -9399,7 +9437,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>283</v>
       </c>
     </row>
@@ -9418,138 +9456,138 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="115" t="s">
         <v>310</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="107">
         <v>1</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108">
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="115" t="s">
         <v>311</v>
       </c>
-      <c r="B6" s="108">
+      <c r="B6" s="107">
         <v>1</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108">
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="115" t="s">
         <v>312</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108">
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107">
         <v>1</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="115" t="s">
         <v>313</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108">
+      <c r="B8" s="107"/>
+      <c r="C8" s="107">
         <v>1</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108">
+      <c r="D8" s="107"/>
+      <c r="E8" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="115" t="s">
         <v>314</v>
       </c>
-      <c r="B9" s="108">
+      <c r="B9" s="107">
         <v>2</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108">
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="115" t="s">
         <v>315</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108">
+      <c r="B10" s="107"/>
+      <c r="C10" s="107">
         <v>1</v>
       </c>
-      <c r="D10" s="108">
+      <c r="D10" s="107">
         <v>1</v>
       </c>
-      <c r="E10" s="108">
+      <c r="E10" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="115" t="s">
         <v>316</v>
       </c>
-      <c r="B11" s="108">
+      <c r="B11" s="107">
         <v>1</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108">
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="115" t="s">
         <v>317</v>
       </c>
-      <c r="B12" s="108">
+      <c r="B12" s="107">
         <v>1</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108">
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="115" t="s">
         <v>318</v>
       </c>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108">
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107">
         <v>1</v>
       </c>
-      <c r="E13" s="108">
+      <c r="E13" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="115" t="s">
         <v>246</v>
       </c>
-      <c r="B14" s="108">
+      <c r="B14" s="107">
         <v>6</v>
       </c>
-      <c r="C14" s="108">
+      <c r="C14" s="107">
         <v>2</v>
       </c>
-      <c r="D14" s="108">
+      <c r="D14" s="107">
         <v>3</v>
       </c>
-      <c r="E14" s="108">
+      <c r="E14" s="107">
         <v>11</v>
       </c>
     </row>
@@ -9989,16 +10027,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="104" t="s">
         <v>247</v>
       </c>
     </row>
@@ -10017,138 +10055,138 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <v>9</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D7" s="107">
         <v>4</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="107">
         <v>6</v>
       </c>
-      <c r="F7" s="108">
+      <c r="F7" s="107">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>4</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D8" s="107">
         <v>3</v>
       </c>
-      <c r="E8" s="108">
+      <c r="E8" s="107">
         <v>3</v>
       </c>
-      <c r="F8" s="108">
+      <c r="F8" s="107">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="107">
         <v>8</v>
       </c>
-      <c r="D9" s="108">
+      <c r="D9" s="107">
         <v>5</v>
       </c>
-      <c r="E9" s="108">
+      <c r="E9" s="107">
         <v>7</v>
       </c>
-      <c r="F9" s="108">
+      <c r="F9" s="107">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="107">
         <v>4</v>
       </c>
-      <c r="D10" s="108">
+      <c r="D10" s="107">
         <v>7</v>
       </c>
-      <c r="E10" s="108">
+      <c r="E10" s="107">
         <v>5</v>
       </c>
-      <c r="F10" s="108">
+      <c r="F10" s="107">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="108">
+      <c r="C11" s="107">
         <v>3</v>
       </c>
-      <c r="D11" s="108">
+      <c r="D11" s="107">
         <v>8</v>
       </c>
-      <c r="E11" s="108">
+      <c r="E11" s="107">
         <v>4</v>
       </c>
-      <c r="F11" s="108">
+      <c r="F11" s="107">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="108">
+      <c r="C12" s="107">
         <v>8</v>
       </c>
-      <c r="D12" s="108">
+      <c r="D12" s="107">
         <v>6</v>
       </c>
-      <c r="E12" s="108">
+      <c r="E12" s="107">
         <v>2</v>
       </c>
-      <c r="F12" s="108">
+      <c r="F12" s="107">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="108">
+      <c r="C13" s="107">
         <v>4</v>
       </c>
-      <c r="D13" s="108">
+      <c r="D13" s="107">
         <v>6</v>
       </c>
-      <c r="E13" s="108">
+      <c r="E13" s="107">
         <v>5</v>
       </c>
-      <c r="F13" s="108">
+      <c r="F13" s="107">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="105" t="s">
         <v>246</v>
       </c>
-      <c r="C14" s="108">
+      <c r="C14" s="107">
         <v>40</v>
       </c>
-      <c r="D14" s="108">
+      <c r="D14" s="107">
         <v>39</v>
       </c>
-      <c r="E14" s="108">
+      <c r="E14" s="107">
         <v>32</v>
       </c>
-      <c r="F14" s="108">
+      <c r="F14" s="107">
         <v>111</v>
       </c>
     </row>
@@ -10177,15 +10215,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="A2" s="111"/>
-      <c r="B2" s="111" t="s">
+      <c r="A2" s="109"/>
+      <c r="B2" s="109" t="s">
         <v>285</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -10199,114 +10237,114 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="107">
         <v>1209.5368600723618</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="107">
         <v>2404.0484175351294</v>
       </c>
-      <c r="D4" s="108">
+      <c r="D4" s="107">
         <v>781.31573569891702</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="106" t="s">
+      <c r="A5" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="107">
         <v>1572.6483398042303</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="107">
         <v>2554.301443631075</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D5" s="107">
         <v>901.5181565756734</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="105" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="108">
+      <c r="B6" s="107">
         <v>1652.7832870554014</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="107">
         <v>1652.7832870554014</v>
       </c>
-      <c r="D6" s="108">
+      <c r="D6" s="107">
         <v>1652.7832870554014</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="108">
+      <c r="B7" s="107">
         <v>1833.0869183705361</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <v>3005.0605219189115</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D7" s="107">
         <v>661.11331482216053</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="108">
+      <c r="B8" s="107">
         <v>1502.5302609594557</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>1502.5302609594557</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D8" s="107">
         <v>1502.5302609594557</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="106" t="s">
+      <c r="A9" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="108">
+      <c r="B9" s="107">
         <v>1752.951971119365</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="107">
         <v>2404.0484175351294</v>
       </c>
-      <c r="D9" s="108">
+      <c r="D9" s="107">
         <v>1352.2772348635101</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="105" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B10" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="D10" s="108">
+      <c r="D10" s="107">
         <v>1803.0363131513468</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="105" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="108">
+      <c r="B11" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="C11" s="108">
+      <c r="C11" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="D11" s="108">
+      <c r="D11" s="107">
         <v>1803.0363131513468</v>
       </c>
     </row>
@@ -10348,27 +10386,27 @@
       <c r="B4" t="s">
         <v>269</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="117" t="s">
         <v>272</v>
       </c>
       <c r="D4" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="108">
+      <c r="E4" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="F4" s="108">
+      <c r="F4" s="107">
         <v>1803.0363131513468</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="117" t="s">
         <v>299</v>
       </c>
-      <c r="E5" s="108">
+      <c r="E5" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="F5" s="108">
+      <c r="F5" s="107">
         <v>1803.0363131513468</v>
       </c>
     </row>
@@ -10379,27 +10417,27 @@
       <c r="B6" t="s">
         <v>288</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="117" t="s">
         <v>289</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="108">
+      <c r="E6" s="107">
         <v>1262.1254192059428</v>
       </c>
-      <c r="F6" s="108">
+      <c r="F6" s="107">
         <v>1262.1254192059428</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="C7" s="119" t="s">
+      <c r="C7" s="117" t="s">
         <v>300</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="107">
         <v>1262.1254192059428</v>
       </c>
-      <c r="F7" s="108">
+      <c r="F7" s="107">
         <v>1262.1254192059428</v>
       </c>
     </row>
@@ -10410,27 +10448,27 @@
       <c r="B8" t="s">
         <v>273</v>
       </c>
-      <c r="C8" s="119" t="s">
+      <c r="C8" s="117" t="s">
         <v>275</v>
       </c>
       <c r="D8" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="108">
+      <c r="E8" s="107">
         <v>3005.0605219189115</v>
       </c>
-      <c r="F8" s="108">
+      <c r="F8" s="107">
         <v>3005.0605219189115</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="117" t="s">
         <v>301</v>
       </c>
-      <c r="E9" s="108">
+      <c r="E9" s="107">
         <v>3005.0605219189115</v>
       </c>
-      <c r="F9" s="108">
+      <c r="F9" s="107">
         <v>3005.0605219189115</v>
       </c>
     </row>
@@ -10438,27 +10476,27 @@
       <c r="B10" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="117" t="s">
         <v>289</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="108">
+      <c r="E10" s="107">
         <v>811.36634091810606</v>
       </c>
-      <c r="F10" s="108">
+      <c r="F10" s="107">
         <v>811.36634091810606</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="117" t="s">
         <v>300</v>
       </c>
-      <c r="E11" s="108">
+      <c r="E11" s="107">
         <v>811.36634091810606</v>
       </c>
-      <c r="F11" s="108">
+      <c r="F11" s="107">
         <v>811.36634091810606</v>
       </c>
     </row>
@@ -10469,27 +10507,27 @@
       <c r="B12" t="s">
         <v>269</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="117" t="s">
         <v>279</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="108">
+      <c r="E12" s="107">
         <v>1352.2772348635101</v>
       </c>
-      <c r="F12" s="108">
+      <c r="F12" s="107">
         <v>1352.2772348635101</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="117" t="s">
         <v>302</v>
       </c>
-      <c r="E13" s="108">
+      <c r="E13" s="107">
         <v>1352.2772348635101</v>
       </c>
-      <c r="F13" s="108">
+      <c r="F13" s="107">
         <v>1352.2772348635101</v>
       </c>
     </row>
@@ -10497,27 +10535,27 @@
       <c r="B14" t="s">
         <v>276</v>
       </c>
-      <c r="C14" s="119" t="s">
+      <c r="C14" s="117" t="s">
         <v>280</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="108">
+      <c r="E14" s="107">
         <v>2404.0484175351294</v>
       </c>
-      <c r="F14" s="108">
+      <c r="F14" s="107">
         <v>2404.0484175351294</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="C15" s="119" t="s">
+      <c r="C15" s="117" t="s">
         <v>303</v>
       </c>
-      <c r="E15" s="108">
+      <c r="E15" s="107">
         <v>2404.0484175351294</v>
       </c>
-      <c r="F15" s="108">
+      <c r="F15" s="107">
         <v>2404.0484175351294</v>
       </c>
     </row>
@@ -10528,27 +10566,27 @@
       <c r="B16" t="s">
         <v>269</v>
       </c>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="117" t="s">
         <v>270</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="108">
+      <c r="E16" s="107">
         <v>781.31573569891702</v>
       </c>
-      <c r="F16" s="108">
+      <c r="F16" s="107">
         <v>781.31573569891702</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="C17" s="119" t="s">
+      <c r="C17" s="117" t="s">
         <v>304</v>
       </c>
-      <c r="E17" s="108">
+      <c r="E17" s="107">
         <v>781.31573569891702</v>
       </c>
-      <c r="F17" s="108">
+      <c r="F17" s="107">
         <v>781.31573569891702</v>
       </c>
     </row>
@@ -10559,27 +10597,27 @@
       <c r="B18" t="s">
         <v>288</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="117" t="s">
         <v>294</v>
       </c>
       <c r="D18" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="108">
+      <c r="E18" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="F18" s="108">
+      <c r="F18" s="107">
         <v>1803.0363131513468</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="117" t="s">
         <v>305</v>
       </c>
-      <c r="E19" s="108">
+      <c r="E19" s="107">
         <v>1803.0363131513468</v>
       </c>
-      <c r="F19" s="108">
+      <c r="F19" s="107">
         <v>1803.0363131513468</v>
       </c>
     </row>
@@ -10590,27 +10628,27 @@
       <c r="B20" t="s">
         <v>269</v>
       </c>
-      <c r="C20" s="119" t="s">
+      <c r="C20" s="117" t="s">
         <v>270</v>
       </c>
       <c r="D20" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="108">
+      <c r="E20" s="107">
         <v>661.11331482216053</v>
       </c>
-      <c r="F20" s="108">
+      <c r="F20" s="107">
         <v>661.11331482216053</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="C21" s="119" t="s">
+      <c r="C21" s="117" t="s">
         <v>304</v>
       </c>
-      <c r="E21" s="108">
+      <c r="E21" s="107">
         <v>661.11331482216053</v>
       </c>
-      <c r="F21" s="108">
+      <c r="F21" s="107">
         <v>661.11331482216053</v>
       </c>
     </row>
@@ -10618,27 +10656,27 @@
       <c r="B22" t="s">
         <v>276</v>
       </c>
-      <c r="C22" s="119" t="s">
+      <c r="C22" s="117" t="s">
         <v>277</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="108">
+      <c r="E22" s="107">
         <v>1502.5302609594557</v>
       </c>
-      <c r="F22" s="108">
+      <c r="F22" s="107">
         <v>1502.5302609594557</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="C23" s="119" t="s">
+      <c r="C23" s="117" t="s">
         <v>306</v>
       </c>
-      <c r="E23" s="108">
+      <c r="E23" s="107">
         <v>1502.5302609594557</v>
       </c>
-      <c r="F23" s="108">
+      <c r="F23" s="107">
         <v>1502.5302609594557</v>
       </c>
     </row>
@@ -10649,27 +10687,27 @@
       <c r="B24" t="s">
         <v>273</v>
       </c>
-      <c r="C24" s="119" t="s">
+      <c r="C24" s="117" t="s">
         <v>274</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="108">
+      <c r="E24" s="107">
         <v>2404.0484175351294</v>
       </c>
-      <c r="F24" s="108">
+      <c r="F24" s="107">
         <v>2404.0484175351294</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="C25" s="119" t="s">
+      <c r="C25" s="117" t="s">
         <v>307</v>
       </c>
-      <c r="E25" s="108">
+      <c r="E25" s="107">
         <v>2404.0484175351294</v>
       </c>
-      <c r="F25" s="108">
+      <c r="F25" s="107">
         <v>2404.0484175351294</v>
       </c>
     </row>
@@ -10677,27 +10715,27 @@
       <c r="B26" t="s">
         <v>288</v>
       </c>
-      <c r="C26" s="119" t="s">
+      <c r="C26" s="117" t="s">
         <v>289</v>
       </c>
       <c r="D26" t="s">
         <v>126</v>
       </c>
-      <c r="E26" s="108">
+      <c r="E26" s="107">
         <v>1652.7832870554014</v>
       </c>
-      <c r="F26" s="108">
+      <c r="F26" s="107">
         <v>1652.7832870554014</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="C27" s="119" t="s">
+      <c r="C27" s="117" t="s">
         <v>300</v>
       </c>
-      <c r="E27" s="108">
+      <c r="E27" s="107">
         <v>1652.7832870554014</v>
       </c>
-      <c r="F27" s="108">
+      <c r="F27" s="107">
         <v>1652.7832870554014</v>
       </c>
     </row>
@@ -10708,27 +10746,27 @@
       <c r="B28" t="s">
         <v>269</v>
       </c>
-      <c r="C28" s="119" t="s">
+      <c r="C28" s="117" t="s">
         <v>270</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="108">
+      <c r="E28" s="107">
         <v>2554.301443631075</v>
       </c>
-      <c r="F28" s="108">
+      <c r="F28" s="107">
         <v>2554.301443631075</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="C29" s="119" t="s">
+      <c r="C29" s="117" t="s">
         <v>304</v>
       </c>
-      <c r="E29" s="108">
+      <c r="E29" s="107">
         <v>2554.301443631075</v>
       </c>
-      <c r="F29" s="108">
+      <c r="F29" s="107">
         <v>2554.301443631075</v>
       </c>
     </row>
@@ -10736,27 +10774,27 @@
       <c r="B30" t="s">
         <v>273</v>
       </c>
-      <c r="C30" s="119" t="s">
+      <c r="C30" s="117" t="s">
         <v>275</v>
       </c>
       <c r="D30" t="s">
         <v>133</v>
       </c>
-      <c r="E30" s="108">
+      <c r="E30" s="107">
         <v>1502.5302609594557</v>
       </c>
-      <c r="F30" s="108">
+      <c r="F30" s="107">
         <v>1502.5302609594557</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="C31" s="119" t="s">
+      <c r="C31" s="117" t="s">
         <v>301</v>
       </c>
-      <c r="E31" s="108">
+      <c r="E31" s="107">
         <v>1502.5302609594557</v>
       </c>
-      <c r="F31" s="108">
+      <c r="F31" s="107">
         <v>1502.5302609594557</v>
       </c>
     </row>
@@ -10767,16 +10805,16 @@
       <c r="B32" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="119" t="s">
+      <c r="C32" s="117" t="s">
         <v>272</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="108">
+      <c r="E32" s="107">
         <v>841.41694613729521</v>
       </c>
-      <c r="F32" s="108">
+      <c r="F32" s="107">
         <v>841.41694613729521</v>
       </c>
     </row>
@@ -10784,21 +10822,21 @@
       <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="108">
+      <c r="E33" s="107">
         <v>901.5181565756734</v>
       </c>
-      <c r="F33" s="108">
+      <c r="F33" s="107">
         <v>901.5181565756734</v>
       </c>
     </row>
     <row r="34" spans="3:6">
-      <c r="C34" s="119" t="s">
+      <c r="C34" s="117" t="s">
         <v>299</v>
       </c>
-      <c r="E34" s="108">
+      <c r="E34" s="107">
         <v>901.5181565756734</v>
       </c>
-      <c r="F34" s="108">
+      <c r="F34" s="107">
         <v>841.41694613729521</v>
       </c>
     </row>
@@ -11807,44 +11845,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="119" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="G2" s="110" t="s">
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="G2" s="119" t="s">
         <v>321</v>
       </c>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="116" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="116" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="118" t="s">
+      <c r="G3" s="116" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="118" t="s">
+      <c r="H3" s="116" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="116" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="116" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="116" t="s">
         <v>157</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="H4" s="116" t="s">
         <v>320</v>
       </c>
     </row>
@@ -11891,48 +11929,48 @@
     </row>
     <row r="8" spans="1:10"/>
     <row r="10" spans="1:10">
-      <c r="G10" s="110" t="s">
+      <c r="G10" s="119" t="s">
         <v>322</v>
       </c>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="G11" s="118" t="s">
+      <c r="G11" s="116" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="118" t="s">
+      <c r="H11" s="116" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="119" t="s">
         <v>309</v>
       </c>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="G12" s="118" t="s">
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="G12" s="116" t="s">
         <v>323</v>
       </c>
-      <c r="H12" s="118" t="s">
+      <c r="H12" s="116" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="116" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="116" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickTop="1">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="116" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="116" t="s">
         <v>183</v>
       </c>
       <c r="G14" s="50" t="s">
@@ -12057,12 +12095,12 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="119" t="s">
         <v>319</v>
       </c>
-      <c r="B21" s="110"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
       <c r="G21" s="54" t="s">
         <v>164</v>
       </c>
@@ -12077,7 +12115,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75">
-      <c r="A22" s="118" t="s">
+      <c r="A22" s="116" t="s">
         <v>100</v>
       </c>
       <c r="G22" s="54" t="s">
@@ -12094,7 +12132,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75">
-      <c r="A23" s="118" t="s">
+      <c r="A23" s="116" t="s">
         <v>320</v>
       </c>
       <c r="G23" s="54" t="s">
@@ -12138,12 +12176,12 @@
       <c r="D26" s="56">
         <v>195710</v>
       </c>
-      <c r="G26" s="110" t="s">
+      <c r="G26" s="119" t="s">
         <v>325</v>
       </c>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="119"/>
     </row>
     <row r="27" spans="1:10" ht="15.75">
       <c r="A27" s="57" t="s">
@@ -12158,10 +12196,10 @@
       <c r="D27" s="59">
         <v>184700</v>
       </c>
-      <c r="G27" s="118" t="s">
+      <c r="G27" s="116" t="s">
         <v>100</v>
       </c>
-      <c r="H27" s="118"/>
+      <c r="H27" s="116"/>
     </row>
     <row r="28" spans="1:10" ht="15.75">
       <c r="A28" s="54" t="s">
@@ -12176,7 +12214,7 @@
       <c r="D28" s="56">
         <v>222050</v>
       </c>
-      <c r="G28" s="118" t="s">
+      <c r="G28" s="116" t="s">
         <v>326</v>
       </c>
     </row>
@@ -12193,7 +12231,7 @@
       <c r="D29" s="59">
         <v>232520</v>
       </c>
-      <c r="G29" s="118" t="s">
+      <c r="G29" s="116" t="s">
         <v>327</v>
       </c>
     </row>
@@ -12604,12 +12642,12 @@
     <row r="52" spans="1:4" ht="13.5" thickTop="1"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G26:J26"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13466,40 +13504,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="119" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="H2" s="110" t="s">
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="H2" s="119" t="s">
         <v>333</v>
       </c>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="116" t="s">
         <v>329</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="H3" s="118" t="s">
+      <c r="B3" s="116"/>
+      <c r="H3" s="116" t="s">
         <v>329</v>
       </c>
-      <c r="I3" s="118" t="s">
+      <c r="I3" s="116" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="116" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="H4" s="118" t="s">
+      <c r="B4" s="116"/>
+      <c r="H4" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="116" t="s">
         <v>335</v>
       </c>
     </row>
@@ -13624,24 +13662,24 @@
     </row>
     <row r="11" spans="1:13" ht="13.5" thickTop="1"/>
     <row r="12" spans="1:13">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="119" t="s">
         <v>330</v>
       </c>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="116" t="s">
         <v>331</v>
       </c>
-      <c r="B13" s="118"/>
+      <c r="B13" s="116"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="116" t="s">
         <v>332</v>
       </c>
-      <c r="B14" s="118"/>
+      <c r="B14" s="116"/>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:13" ht="13.5" thickTop="1">
@@ -13906,24 +13944,24 @@
     </row>
     <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
     <row r="30" spans="1:6">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="119" t="s">
         <v>333</v>
       </c>
-      <c r="B30" s="110"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="118" t="s">
+      <c r="A31" s="116" t="s">
         <v>334</v>
       </c>
-      <c r="B31" s="118"/>
+      <c r="B31" s="116"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="118" t="s">
+      <c r="A32" s="116" t="s">
         <v>335</v>
       </c>
-      <c r="B32" s="118"/>
+      <c r="B32" s="116"/>
     </row>
     <row r="33" spans="1:6" ht="13.5" thickBot="1"/>
     <row r="34" spans="1:6" ht="13.5" thickTop="1">
@@ -14396,45 +14434,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="119" t="s">
         <v>336</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="F2" s="110" t="s">
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="F2" s="119" t="s">
         <v>342</v>
       </c>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="L2" s="110" t="s">
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="L2" s="119" t="s">
         <v>345</v>
       </c>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickTop="1">
       <c r="A3" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="F3" s="118" t="s">
+      <c r="F3" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="L3" s="118" t="s">
+      <c r="L3" s="116" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="118">
+      <c r="A4" s="116">
         <f>MIN('8'!C2:C16)</f>
         <v>22</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="L4" s="118" t="s">
+      <c r="L4" s="116" t="s">
         <v>346</v>
       </c>
     </row>
@@ -14538,12 +14576,12 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="119" t="s">
         <v>336</v>
       </c>
-      <c r="B10" s="110"/>
-      <c r="C10" s="110"/>
-      <c r="D10" s="110"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
       <c r="F10" s="87" t="s">
         <v>218</v>
       </c>
@@ -14569,19 +14607,19 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="118">
+      <c r="A12" s="116">
         <f>MAX('8'!C2:C16)</f>
         <v>375</v>
       </c>
-      <c r="F12" s="110" t="s">
+      <c r="F12" s="119" t="s">
         <v>343</v>
       </c>
-      <c r="G12" s="110"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
     </row>
     <row r="13" spans="1:15" ht="13.5" thickBot="1">
-      <c r="F13" s="118" t="s">
+      <c r="F13" s="116" t="s">
         <v>198</v>
       </c>
     </row>
@@ -14595,7 +14633,7 @@
       <c r="C14" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="F14" s="118" t="s">
+      <c r="F14" s="116" t="s">
         <v>207</v>
       </c>
     </row>
@@ -14645,12 +14683,12 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="110" t="s">
+      <c r="A20" s="119" t="s">
         <v>337</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
       <c r="F20" s="80" t="s">
         <v>216</v>
       </c>
@@ -14662,23 +14700,23 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="116" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="118" t="s">
+      <c r="A22" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="F22" s="110" t="s">
+      <c r="F22" s="119" t="s">
         <v>344</v>
       </c>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
     </row>
     <row r="23" spans="1:9" ht="13.5" thickBot="1">
-      <c r="F23" s="118" t="s">
+      <c r="F23" s="116" t="s">
         <v>198</v>
       </c>
     </row>
@@ -14692,7 +14730,7 @@
       <c r="C24" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="F24" s="118" t="s">
+      <c r="F24" s="116" t="s">
         <v>204</v>
       </c>
     </row>
@@ -14779,26 +14817,26 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="119" t="s">
         <v>338</v>
       </c>
-      <c r="B30" s="110"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="118" t="s">
+      <c r="A31" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="B31" s="118" t="s">
+      <c r="B31" s="116" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="118" t="s">
+      <c r="A32" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="B32" s="118" t="s">
+      <c r="B32" s="116" t="s">
         <v>339</v>
       </c>
     </row>
@@ -14826,24 +14864,24 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="110" t="s">
+      <c r="A37" s="119" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="110"/>
-      <c r="C37" s="110"/>
-      <c r="D37" s="110"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="119"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="118" t="s">
+      <c r="A38" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="B38" s="118"/>
+      <c r="B38" s="116"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="118" t="s">
+      <c r="A39" s="116" t="s">
         <v>341</v>
       </c>
-      <c r="B39" s="118"/>
+      <c r="B39" s="116"/>
     </row>
     <row r="40" spans="1:4" ht="13.5" thickBot="1"/>
     <row r="41" spans="1:4" ht="13.5" thickTop="1">
@@ -14980,15 +15018,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F22:I22"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15002,7 +15040,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="A1:F11"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -15497,64 +15535,64 @@
         <v>871.47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25">
+    <row r="3" spans="1:6" ht="14.25" hidden="1">
       <c r="A3" s="91" t="s">
-        <v>225</v>
+        <v>39</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C3" s="92">
-        <v>35441</v>
+        <v>35440</v>
       </c>
       <c r="D3" s="91" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="F3" s="93">
-        <v>1502.53</v>
+        <v>21035.42</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="91" t="s">
-        <v>39</v>
+        <v>241</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="C4" s="92">
-        <v>35440</v>
+        <v>35473</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4" s="91" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="F4" s="93">
-        <v>721.21</v>
+        <v>1472.48</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="91" t="s">
-        <v>39</v>
+        <v>225</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C5" s="92">
-        <v>35440</v>
+        <v>35441</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" s="91" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F5" s="93">
-        <v>21035.42</v>
+        <v>1502.53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" hidden="1">
@@ -15597,7 +15635,7 @@
         <v>1724.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25">
+    <row r="8" spans="1:6" ht="14.25" hidden="1">
       <c r="A8" s="91" t="s">
         <v>236</v>
       </c>
@@ -15657,37 +15695,36 @@
         <v>2151.62</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1">
+    <row r="11" spans="1:6" ht="15" hidden="1" thickBot="1">
       <c r="A11" s="94" t="s">
-        <v>241</v>
+        <v>39</v>
       </c>
       <c r="B11" s="94" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C11" s="95">
-        <v>35473</v>
+        <v>35440</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="F11" s="96">
-        <v>1472.48</v>
+        <v>721.21</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F11">
     <filterColumn colId="3">
       <filters>
-        <filter val="Centro"/>
         <filter val="Sur"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="5">
-      <top10 val="10" filterVal="721.21"/>
-    </filterColumn>
+    <sortState ref="A4:F7">
+      <sortCondition ref="F1:F11"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="76" orientation="portrait" cellComments="asDisplayed" r:id="rId1"/>
@@ -15700,35 +15737,36 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N25"/>
+  <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="119" t="s">
         <v>347</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="I2" s="110" t="s">
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="I2" s="119" t="s">
         <v>349</v>
       </c>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
       <c r="A3" s="90" t="s">
@@ -15739,15 +15777,15 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="116" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="13.5" thickBot="1">
-      <c r="I5" s="118" t="s">
+      <c r="I5" s="116" t="s">
         <v>15</v>
       </c>
     </row>
@@ -15944,12 +15982,12 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="119" t="s">
         <v>348</v>
       </c>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
       <c r="I12" s="91" t="s">
         <v>60</v>
       </c>
@@ -15996,10 +16034,10 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="118" t="e">
+      <c r="B14" s="116" t="e">
         <f>VLOOKUP(A14,'9'!A1:F11,6,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -16043,16 +16081,34 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="9:14">
-      <c r="I17" s="110" t="s">
+    <row r="17" spans="1:14" ht="14.25">
+      <c r="A17" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" s="92">
+        <v>35473</v>
+      </c>
+      <c r="D17" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="91" t="s">
+        <v>240</v>
+      </c>
+      <c r="F17" s="93">
+        <v>2752.64</v>
+      </c>
+      <c r="I17" s="119" t="s">
         <v>350</v>
       </c>
-      <c r="J17" s="110"/>
-      <c r="K17" s="110"/>
-      <c r="L17" s="110"/>
-    </row>
-    <row r="18" spans="9:14" ht="13.5" thickBot="1"/>
-    <row r="19" spans="9:14" ht="15.75">
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+    </row>
+    <row r="18" spans="1:14" ht="13.5" thickBot="1"/>
+    <row r="19" spans="1:14" ht="15.75">
       <c r="I19" s="90" t="s">
         <v>1</v>
       </c>
@@ -16072,7 +16128,13 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="9:14" ht="14.25">
+    <row r="20" spans="1:14" ht="14.25">
+      <c r="A20" s="119" t="s">
+        <v>351</v>
+      </c>
+      <c r="B20" s="119"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
       <c r="I20" s="91" t="s">
         <v>225</v>
       </c>
@@ -16092,7 +16154,7 @@
         <v>1502.53</v>
       </c>
     </row>
-    <row r="21" spans="9:14" ht="14.25">
+    <row r="21" spans="1:14" ht="15" thickBot="1">
       <c r="I21" s="91" t="s">
         <v>39</v>
       </c>
@@ -16112,7 +16174,25 @@
         <v>721.21</v>
       </c>
     </row>
-    <row r="22" spans="9:14" ht="14.25">
+    <row r="22" spans="1:14" ht="15.75">
+      <c r="A22" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="90" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="90" t="s">
+        <v>220</v>
+      </c>
+      <c r="E22" s="90" t="s">
+        <v>221</v>
+      </c>
+      <c r="F22" s="90" t="s">
+        <v>222</v>
+      </c>
       <c r="I22" s="91" t="s">
         <v>39</v>
       </c>
@@ -16132,7 +16212,25 @@
         <v>21035.42</v>
       </c>
     </row>
-    <row r="23" spans="9:14" ht="14.25">
+    <row r="23" spans="1:14" ht="14.25">
+      <c r="A23" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="91" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="92">
+        <v>35440</v>
+      </c>
+      <c r="D23" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="91" t="s">
+        <v>231</v>
+      </c>
+      <c r="F23" s="93">
+        <v>21035.42</v>
+      </c>
       <c r="I23" s="91" t="s">
         <v>235</v>
       </c>
@@ -16152,7 +16250,25 @@
         <v>1724.9</v>
       </c>
     </row>
-    <row r="24" spans="9:14" ht="14.25">
+    <row r="24" spans="1:14" ht="14.25">
+      <c r="A24" s="91" t="s">
+        <v>235</v>
+      </c>
+      <c r="B24" s="91" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" s="92">
+        <v>35472</v>
+      </c>
+      <c r="D24" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="F24" s="93">
+        <v>1724.9</v>
+      </c>
       <c r="I24" s="91" t="s">
         <v>236</v>
       </c>
@@ -16172,7 +16288,25 @@
         <v>901.52</v>
       </c>
     </row>
-    <row r="25" spans="9:14" ht="15" thickBot="1">
+    <row r="25" spans="1:14" ht="15" thickBot="1">
+      <c r="A25" s="91" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="C25" s="92">
+        <v>35441</v>
+      </c>
+      <c r="D25" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="F25" s="93">
+        <v>1502.53</v>
+      </c>
       <c r="I25" s="94" t="s">
         <v>241</v>
       </c>
@@ -16192,12 +16326,143 @@
         <v>1472.48</v>
       </c>
     </row>
+    <row r="26" spans="1:14" ht="14.25">
+      <c r="A26" s="91" t="s">
+        <v>241</v>
+      </c>
+      <c r="B26" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="92">
+        <v>35473</v>
+      </c>
+      <c r="D26" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="91" t="s">
+        <v>245</v>
+      </c>
+      <c r="F26" s="93">
+        <v>1472.48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="14.25">
+      <c r="A27" s="91" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" s="91" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" s="92">
+        <v>35475</v>
+      </c>
+      <c r="D27" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="91" t="s">
+        <v>238</v>
+      </c>
+      <c r="F27" s="93">
+        <v>901.52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15" thickBot="1">
+      <c r="A28" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="94" t="s">
+        <v>228</v>
+      </c>
+      <c r="C28" s="95">
+        <v>35440</v>
+      </c>
+      <c r="D28" s="94" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="F28" s="96">
+        <v>721.21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="119" t="s">
+        <v>352</v>
+      </c>
+      <c r="B31" s="119"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="119"/>
+    </row>
+    <row r="32" spans="1:14" ht="13.5" thickBot="1"/>
+    <row r="33" spans="1:6" ht="15.75">
+      <c r="A33" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="90" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="90" t="s">
+        <v>220</v>
+      </c>
+      <c r="E33" s="90" t="s">
+        <v>221</v>
+      </c>
+      <c r="F33" s="90" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.25">
+      <c r="A34" s="91" t="s">
+        <v>241</v>
+      </c>
+      <c r="B34" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="C34" s="92">
+        <v>35473</v>
+      </c>
+      <c r="D34" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="91" t="s">
+        <v>245</v>
+      </c>
+      <c r="F34" s="93">
+        <v>1472.48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.25">
+      <c r="A35" s="91" t="s">
+        <v>225</v>
+      </c>
+      <c r="B35" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" s="92">
+        <v>35441</v>
+      </c>
+      <c r="D35" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="F35" s="93">
+        <v>1502.53</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="I17:L17"/>
+    <mergeCell ref="A20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16218,118 +16483,118 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="119" t="s">
         <v>248</v>
       </c>
-      <c r="C3" s="110"/>
+      <c r="C3" s="119"/>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="109"/>
-      <c r="C5" s="109" t="s">
+      <c r="B5" s="108"/>
+      <c r="C5" s="108" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="107">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="107">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="107">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="108">
+      <c r="C11" s="107">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="108">
+      <c r="C12" s="107">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="108">
+      <c r="C13" s="107">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="108">
+      <c r="C14" s="107">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="108">
+      <c r="C15" s="107">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="108">
+      <c r="C16" s="107">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="108">
+      <c r="C17" s="107">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="105" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="108">
+      <c r="C18" s="107">
         <v>111</v>
       </c>
     </row>
@@ -16343,10 +16608,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:H40"/>
+  <dimension ref="A7:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -16354,7 +16619,7 @@
     <col min="1" max="16384" width="11.42578125" style="63"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:8" ht="30.75" customHeight="1">
+    <row r="7" spans="1:17" ht="30.75" customHeight="1">
       <c r="A7" s="97" t="s">
         <v>94</v>
       </c>
@@ -16378,7 +16643,7 @@
       </c>
       <c r="H7" s="99"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:17">
       <c r="A8" s="100">
         <v>38718</v>
       </c>
@@ -16401,7 +16666,7 @@
         <v>149.05000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:17">
       <c r="A9" s="100">
         <v>38444</v>
       </c>
@@ -16423,8 +16688,14 @@
       <c r="G9" s="103">
         <v>143.63999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="K9" s="119" t="s">
+        <v>356</v>
+      </c>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="100">
         <v>38585</v>
       </c>
@@ -16446,8 +16717,11 @@
       <c r="G10" s="103">
         <v>131.02000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="K10" s="118" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="100">
         <v>37987</v>
       </c>
@@ -16469,8 +16743,14 @@
       <c r="G11" s="103">
         <v>117.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="K11" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="100">
         <v>38408</v>
       </c>
@@ -16492,8 +16772,14 @@
       <c r="G12" s="103">
         <v>96.76</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="K12" s="63" t="s">
+        <v>357</v>
+      </c>
+      <c r="L12" s="63" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="100">
         <v>38385</v>
       </c>
@@ -16516,7 +16802,7 @@
         <v>155.06</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:17" ht="25.5">
       <c r="A14" s="100">
         <v>38779</v>
       </c>
@@ -16538,8 +16824,29 @@
       <c r="G14" s="103">
         <v>209.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="K14" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="O14" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="P14" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q14" s="97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="100">
         <v>38933</v>
       </c>
@@ -16561,8 +16868,29 @@
       <c r="G15" s="103">
         <v>250.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="K15" s="100">
+        <v>37987</v>
+      </c>
+      <c r="L15" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="M15" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N15" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="O15" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="P15" s="102">
+        <v>195</v>
+      </c>
+      <c r="Q15" s="103">
+        <v>117.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="100">
         <v>38353</v>
       </c>
@@ -16585,7 +16913,7 @@
         <v>239.2</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:17">
       <c r="A17" s="100">
         <v>38904</v>
       </c>
@@ -16608,7 +16936,7 @@
         <v>185.71</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:17">
       <c r="A18" s="100">
         <v>38509</v>
       </c>
@@ -16630,11 +16958,546 @@
       <c r="G18" s="103">
         <v>185.71</v>
       </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="104"/>
+      <c r="K18" s="119" t="s">
+        <v>359</v>
+      </c>
+      <c r="L18" s="119"/>
+      <c r="M18" s="119"/>
+      <c r="N18" s="119"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="K19" s="118" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="K20" s="63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="119" t="s">
+        <v>353</v>
+      </c>
+      <c r="B21" s="119"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
+      <c r="K21" s="63" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="118" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="25.5">
+      <c r="A23" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="L23" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="M23" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="N23" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="O23" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="P23" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q23" s="97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="100">
+        <v>38385</v>
+      </c>
+      <c r="L24" s="101" t="s">
+        <v>112</v>
+      </c>
+      <c r="M24" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N24" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="O24" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="P24" s="102">
+        <v>258</v>
+      </c>
+      <c r="Q24" s="103">
+        <v>155.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="K25" s="100">
+        <v>38779</v>
+      </c>
+      <c r="L25" s="101" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N25" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="O25" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="P25" s="102">
+        <v>349</v>
+      </c>
+      <c r="Q25" s="103">
+        <v>209.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="25.5">
+      <c r="A26" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="97" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" s="100">
+        <v>38933</v>
+      </c>
+      <c r="L26" s="101" t="s">
+        <v>101</v>
+      </c>
+      <c r="M26" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N26" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="O26" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="P26" s="102">
+        <v>417</v>
+      </c>
+      <c r="Q26" s="103">
+        <v>250.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="100">
+        <v>38444</v>
+      </c>
+      <c r="B27" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="102">
+        <v>239</v>
+      </c>
+      <c r="G27" s="103">
+        <v>143.63999999999999</v>
+      </c>
+      <c r="K27" s="100">
+        <v>38353</v>
+      </c>
+      <c r="L27" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="M27" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="N27" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="O27" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="P27" s="102">
+        <v>398</v>
+      </c>
+      <c r="Q27" s="103">
+        <v>239.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="100">
+        <v>38585</v>
+      </c>
+      <c r="B28" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="102">
+        <v>218</v>
+      </c>
+      <c r="G28" s="103">
+        <v>131.02000000000001</v>
+      </c>
+      <c r="K28" s="100">
+        <v>38904</v>
+      </c>
+      <c r="L28" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="M28" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N28" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="O28" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="P28" s="102">
+        <v>309</v>
+      </c>
+      <c r="Q28" s="103">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="100">
+        <v>38353</v>
+      </c>
+      <c r="B29" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="102">
+        <v>398</v>
+      </c>
+      <c r="G29" s="103">
+        <v>239.2</v>
+      </c>
+      <c r="K29" s="100">
+        <v>38509</v>
+      </c>
+      <c r="L29" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="M29" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N29" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="O29" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="P29" s="102">
+        <v>309</v>
+      </c>
+      <c r="Q29" s="103">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="K31" s="119" t="s">
+        <v>361</v>
+      </c>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="119"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="119" t="s">
+        <v>355</v>
+      </c>
+      <c r="B32" s="119"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="119"/>
+      <c r="K32" s="118" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="118" t="s">
+        <v>354</v>
+      </c>
+      <c r="K33" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="L33" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="M33" s="63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="K34" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="L34" s="63" t="s">
+        <v>362</v>
+      </c>
+      <c r="M34" s="63" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="K35" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="L35" s="63" t="s">
+        <v>362</v>
+      </c>
+      <c r="M35" s="63" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="K36" s="101"/>
+      <c r="L36" s="101"/>
+      <c r="M36" s="101"/>
+      <c r="N36" s="101"/>
+      <c r="O36" s="101"/>
+      <c r="P36" s="101"/>
+      <c r="Q36" s="101"/>
+    </row>
+    <row r="37" spans="1:17" ht="25.5">
+      <c r="A37" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="97" t="s">
+        <v>100</v>
+      </c>
+      <c r="K37" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="L37" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="M37" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="N37" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="O37" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="P37" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q37" s="97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="100">
+        <v>38444</v>
+      </c>
+      <c r="B38" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="102">
+        <v>239</v>
+      </c>
+      <c r="G38" s="103">
+        <v>143.63999999999999</v>
+      </c>
+      <c r="K38" s="100">
+        <v>38353</v>
+      </c>
+      <c r="L38" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="M38" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="N38" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="O38" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="P38" s="102">
+        <v>398</v>
+      </c>
+      <c r="Q38" s="103">
+        <v>239.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="100">
+        <v>38585</v>
+      </c>
+      <c r="B39" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" s="102">
+        <v>218</v>
+      </c>
+      <c r="G39" s="103">
+        <v>131.02000000000001</v>
+      </c>
+      <c r="K39" s="100">
+        <v>38904</v>
+      </c>
+      <c r="L39" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="M39" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="N39" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="O39" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="P39" s="102">
+        <v>309</v>
+      </c>
+      <c r="Q39" s="103">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="100">
+        <v>38353</v>
+      </c>
+      <c r="B40" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" s="102">
+        <v>398</v>
+      </c>
+      <c r="G40" s="103">
+        <v>239.2</v>
+      </c>
+      <c r="K40" s="100"/>
+      <c r="L40" s="101"/>
+      <c r="P40" s="102"/>
+      <c r="Q40" s="103"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="K41" s="100"/>
+      <c r="L41" s="101"/>
+      <c r="P41" s="102"/>
+      <c r="Q41" s="103"/>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="K42" s="100"/>
+      <c r="L42" s="101"/>
+      <c r="P42" s="102"/>
+      <c r="Q42" s="103"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K31:O31"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
@@ -16656,16 +17519,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="119" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="104" t="s">
         <v>247</v>
       </c>
     </row>
@@ -16684,343 +17547,343 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="107">
         <v>25</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D7" s="107">
         <v>7</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="107">
         <v>8</v>
       </c>
-      <c r="F7" s="108">
+      <c r="F7" s="107">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>9</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108">
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108">
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107">
         <v>4</v>
       </c>
-      <c r="F9" s="108">
+      <c r="F9" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="107">
         <v>8</v>
       </c>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108">
+      <c r="D10" s="107"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="107">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108">
+      <c r="C11" s="107"/>
+      <c r="D11" s="107">
         <v>4</v>
       </c>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108">
+      <c r="E11" s="107"/>
+      <c r="F11" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108">
+      <c r="C12" s="107"/>
+      <c r="D12" s="107">
         <v>3</v>
       </c>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108">
+      <c r="E12" s="107"/>
+      <c r="F12" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="108">
+      <c r="C13" s="107">
         <v>8</v>
       </c>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108">
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="108"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="108">
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107">
         <v>4</v>
       </c>
-      <c r="F14" s="108">
+      <c r="F14" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="108">
+      <c r="C15" s="107">
         <v>15</v>
       </c>
-      <c r="D15" s="108">
+      <c r="D15" s="107">
         <v>15</v>
       </c>
-      <c r="E15" s="108">
+      <c r="E15" s="107">
         <v>9</v>
       </c>
-      <c r="F15" s="108">
+      <c r="F15" s="107">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="108">
+      <c r="C16" s="107">
         <v>4</v>
       </c>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108">
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108">
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107">
         <v>3</v>
       </c>
-      <c r="F17" s="108">
+      <c r="F17" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="108">
+      <c r="C18" s="107">
         <v>5</v>
       </c>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108">
+      <c r="D18" s="107"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="107">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108">
+      <c r="C19" s="107"/>
+      <c r="D19" s="107">
         <v>7</v>
       </c>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108">
+      <c r="E19" s="107"/>
+      <c r="F19" s="107">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108">
+      <c r="C20" s="107"/>
+      <c r="D20" s="107">
         <v>8</v>
       </c>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108">
+      <c r="E20" s="107"/>
+      <c r="F20" s="107">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="107" t="s">
+      <c r="B21" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="108">
+      <c r="C21" s="107">
         <v>6</v>
       </c>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108">
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="108"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="108">
+      <c r="C22" s="107"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107">
         <v>6</v>
       </c>
-      <c r="F22" s="108">
+      <c r="F22" s="107">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="108">
+      <c r="C23" s="107">
         <v>15</v>
       </c>
-      <c r="D23" s="108">
+      <c r="D23" s="107">
         <v>9</v>
       </c>
-      <c r="E23" s="108">
+      <c r="E23" s="107">
         <v>8</v>
       </c>
-      <c r="F23" s="108">
+      <c r="F23" s="107">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="107" t="s">
+      <c r="B24" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="108">
+      <c r="C24" s="107">
         <v>6</v>
       </c>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="108">
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108">
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107">
         <v>3</v>
       </c>
-      <c r="F25" s="108">
+      <c r="F25" s="107">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="107" t="s">
+      <c r="B26" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="108">
+      <c r="C26" s="107">
         <v>7</v>
       </c>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="108">
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="107" t="s">
+      <c r="B27" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="108"/>
-      <c r="D27" s="108">
+      <c r="C27" s="107"/>
+      <c r="D27" s="107">
         <v>5</v>
       </c>
-      <c r="E27" s="108"/>
-      <c r="F27" s="108">
+      <c r="E27" s="107"/>
+      <c r="F27" s="107">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="108"/>
-      <c r="D28" s="108">
+      <c r="C28" s="107"/>
+      <c r="D28" s="107">
         <v>4</v>
       </c>
-      <c r="E28" s="108"/>
-      <c r="F28" s="108">
+      <c r="E28" s="107"/>
+      <c r="F28" s="107">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="107" t="s">
+      <c r="B29" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="108">
+      <c r="C29" s="107">
         <v>2</v>
       </c>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108">
+      <c r="D29" s="107"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="107">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="108"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="108">
+      <c r="C30" s="107"/>
+      <c r="D30" s="107"/>
+      <c r="E30" s="107">
         <v>5</v>
       </c>
-      <c r="F30" s="108">
+      <c r="F30" s="107">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:6">
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="105" t="s">
         <v>246</v>
       </c>
-      <c r="C31" s="108">
+      <c r="C31" s="107">
         <v>55</v>
       </c>
-      <c r="D31" s="108">
+      <c r="D31" s="107">
         <v>31</v>
       </c>
-      <c r="E31" s="108">
+      <c r="E31" s="107">
         <v>25</v>
       </c>
-      <c r="F31" s="108">
+      <c r="F31" s="107">
         <v>111</v>
       </c>
     </row>
@@ -17047,16 +17910,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="119" t="s">
         <v>252</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="104" t="s">
         <v>250</v>
       </c>
     </row>
@@ -17075,70 +17938,70 @@
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="112">
+      <c r="C8" s="110">
         <v>8.3333333333333339</v>
       </c>
-      <c r="D8" s="112">
+      <c r="D8" s="110">
         <v>5</v>
       </c>
-      <c r="E8" s="112">
+      <c r="E8" s="110">
         <v>5</v>
       </c>
-      <c r="F8" s="112">
+      <c r="F8" s="110">
         <v>6.1111111111111107</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="112">
+      <c r="C9" s="110">
         <v>3.5</v>
       </c>
-      <c r="D9" s="112">
+      <c r="D9" s="110">
         <v>7.5</v>
       </c>
-      <c r="E9" s="112">
+      <c r="E9" s="110">
         <v>4.5</v>
       </c>
-      <c r="F9" s="112">
+      <c r="F9" s="110">
         <v>5.166666666666667</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="110">
         <v>4</v>
       </c>
-      <c r="D10" s="112">
+      <c r="D10" s="110">
         <v>4.5</v>
       </c>
-      <c r="E10" s="112">
+      <c r="E10" s="110">
         <v>4</v>
       </c>
-      <c r="F10" s="112">
+      <c r="F10" s="110">
         <v>4.166666666666667</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="105" t="s">
         <v>246</v>
       </c>
-      <c r="C11" s="112">
+      <c r="C11" s="110">
         <v>5.7142857142857144</v>
       </c>
-      <c r="D11" s="112">
+      <c r="D11" s="110">
         <v>5.5714285714285712</v>
       </c>
-      <c r="E11" s="112">
+      <c r="E11" s="110">
         <v>4.5714285714285712</v>
       </c>
-      <c r="F11" s="112">
+      <c r="F11" s="110">
         <v>5.2857142857142856</v>
       </c>
     </row>
@@ -17601,12 +18464,12 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:3">
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="104" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="104" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -17617,7 +18480,7 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="107">
         <v>5</v>
       </c>
     </row>
@@ -17625,7 +18488,7 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="107">
         <v>6</v>
       </c>
     </row>
@@ -17633,7 +18496,7 @@
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="107">
         <v>5</v>
       </c>
     </row>
@@ -17658,7 +18521,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>253</v>
       </c>
     </row>
@@ -17677,51 +18540,51 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="113">
+      <c r="B5" s="111">
         <v>1</v>
       </c>
-      <c r="C5" s="113">
+      <c r="C5" s="111">
         <v>3</v>
       </c>
-      <c r="D5" s="113">
+      <c r="D5" s="111">
         <v>1</v>
       </c>
-      <c r="E5" s="113">
+      <c r="E5" s="111">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="113">
+      <c r="B6" s="111">
         <v>1</v>
       </c>
-      <c r="C6" s="113">
+      <c r="C6" s="111">
         <v>2</v>
       </c>
-      <c r="D6" s="113">
+      <c r="D6" s="111">
         <v>3</v>
       </c>
-      <c r="E6" s="113">
+      <c r="E6" s="111">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="114" t="s">
+      <c r="A7" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="113">
+      <c r="B7" s="111">
         <v>4</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113">
+      <c r="C7" s="111"/>
+      <c r="D7" s="111">
         <v>1</v>
       </c>
-      <c r="E7" s="113">
+      <c r="E7" s="111">
         <v>5</v>
       </c>
     </row>
@@ -17760,10 +18623,10 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="112">
+      <c r="B4" s="110">
         <v>5619.4631759883641</v>
       </c>
-      <c r="C4" s="112">
+      <c r="C4" s="110">
         <v>1123.8926351976729</v>
       </c>
     </row>
@@ -17771,10 +18634,10 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="112">
+      <c r="B5" s="110">
         <v>8083.6128039618725</v>
       </c>
-      <c r="C5" s="112">
+      <c r="C5" s="110">
         <v>1347.2688006603121</v>
       </c>
     </row>
@@ -17782,10 +18645,10 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="112">
+      <c r="B6" s="110">
         <v>7783.1067517699803</v>
       </c>
-      <c r="C6" s="112">
+      <c r="C6" s="110">
         <v>1556.6213503539961</v>
       </c>
     </row>

</xml_diff>